<commit_message>
Tudo pronto e A* dando pau em um teste dos 9
</commit_message>
<xml_diff>
--- a/tp1/Resultados.xlsx
+++ b/tp1/Resultados.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\romeu\Documents\repos\AI\tp1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{A614B12B-CDE1-44B5-8D14-6B8BC40A03FE}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{EE70D295-0A1C-41C4-9F4C-35F1FA9CF57F}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{D13A2FBD-B21C-43BE-BD63-69798AA2AB0E}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="51">
   <si>
     <t>Teste 1</t>
   </si>
@@ -151,6 +151,33 @@
   </si>
   <si>
     <t>0.210</t>
+  </si>
+  <si>
+    <t>0.470</t>
+  </si>
+  <si>
+    <t>0.164</t>
+  </si>
+  <si>
+    <t>0.168</t>
+  </si>
+  <si>
+    <t>0.309</t>
+  </si>
+  <si>
+    <t>Manhattan</t>
+  </si>
+  <si>
+    <t>0.174</t>
+  </si>
+  <si>
+    <t>Octile</t>
+  </si>
+  <si>
+    <t>0.260</t>
+  </si>
+  <si>
+    <t>0.160</t>
   </si>
 </sst>
 </file>
@@ -186,8 +213,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -511,304 +541,375 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{960F0236-32BC-43B3-B21D-DBFCEA12ACBB}">
-  <dimension ref="A1:K17"/>
+  <dimension ref="A1:M17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C4" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" topLeftCell="E10" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="3" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="9" style="1" customWidth="1"/>
-    <col min="6" max="6" width="8" style="1" customWidth="1"/>
-    <col min="7" max="7" width="8.42578125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="8.28515625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="9" style="1" customWidth="1"/>
-    <col min="10" max="10" width="7.85546875" style="1" customWidth="1"/>
-    <col min="11" max="11" width="9.140625" style="1"/>
+    <col min="1" max="1" width="9.140625" style="2"/>
+    <col min="2" max="3" width="9.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.140625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="9" style="2" customWidth="1"/>
+    <col min="6" max="6" width="8" style="2" customWidth="1"/>
+    <col min="7" max="7" width="8.42578125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="8.28515625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="9" style="2" customWidth="1"/>
+    <col min="10" max="10" width="7.85546875" style="2" customWidth="1"/>
+    <col min="11" max="11" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D1" s="2" t="s">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2" t="s">
+      <c r="E1" s="3"/>
+      <c r="F1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2" t="s">
+      <c r="G1" s="3"/>
+      <c r="H1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2" t="s">
+      <c r="I1" s="3"/>
+      <c r="J1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="K1" s="2"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B3" s="1" t="s">
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="J2" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="K2" s="3"/>
+      <c r="L2" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="M2" s="1"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="G3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="H3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="I3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="J3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="K3" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="L3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5" s="2">
         <v>213</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="4">
         <v>42640</v>
       </c>
-      <c r="F5" s="1">
+      <c r="F5" s="2">
         <v>213</v>
       </c>
-      <c r="G5" s="3">
+      <c r="G5" s="4">
         <v>1070</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="J5" s="2">
+        <v>213</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6" s="2">
         <v>15</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="F6" s="1">
+      <c r="F6" s="2">
         <v>15</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="G6" s="2" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="J6" s="2">
+        <v>15</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="4">
         <v>208032</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="F7" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="G7" s="3">
+      <c r="G7" s="4">
         <v>2891</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="J7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D10" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10" s="4">
         <v>126493</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="F10" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="G10" s="3">
+      <c r="G10" s="4">
         <v>2542</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+      <c r="J10" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D11" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E11" s="3">
+      <c r="E11" s="4">
         <v>31894</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="F11" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="G11" s="1" t="s">
+      <c r="G11" s="2" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+      <c r="J11" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="L11">
+        <v>140</v>
+      </c>
+      <c r="M11" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D12" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="E12" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="F12" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="G12" s="1" t="s">
+      <c r="G12" s="2" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+      <c r="J12" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C15" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D15" s="1">
+      <c r="D15" s="2">
         <v>435</v>
       </c>
-      <c r="E15" s="3">
+      <c r="E15" s="4">
         <v>516950</v>
       </c>
-      <c r="F15" s="1">
+      <c r="F15" s="2">
         <v>435</v>
       </c>
-      <c r="G15" s="3">
+      <c r="G15" s="4">
         <v>3372</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+      <c r="J15" s="2">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C16" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="D16" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E16" s="3">
+      <c r="E16" s="4">
         <v>409746</v>
       </c>
-      <c r="F16" s="1" t="s">
+      <c r="F16" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="G16" s="3">
+      <c r="G16" s="4">
         <v>3463</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
+      <c r="J16" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C17" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="D17" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E17" s="3">
+      <c r="E17" s="4">
         <v>541500</v>
       </c>
-      <c r="F17" s="1" t="s">
+      <c r="F17" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="G17" s="3">
+      <c r="G17" s="4">
         <v>3369</v>
       </c>
+      <c r="J17" s="2" t="s">
+        <v>21</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="6">
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="F1:G1"/>
     <mergeCell ref="H1:I1"/>
-    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="J1:M1"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="L2:M2"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>